<commit_message>
improve cell and inclusion segmentation algorithm
</commit_message>
<xml_diff>
--- a/PFF_SCR_TAX_ADAM/251024_analysis_by_cell_NEW.xlsx
+++ b/PFF_SCR_TAX_ADAM/251024_analysis_by_cell_NEW.xlsx
@@ -460,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -486,7 +486,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -525,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -551,7 +551,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -577,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -590,7 +590,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -642,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -655,7 +655,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -681,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -694,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -746,7 +746,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
@@ -785,7 +785,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -850,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -876,7 +876,7 @@
         <v>3</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -889,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -902,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -928,7 +928,7 @@
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -967,7 +967,7 @@
         <v>2</v>
       </c>
       <c r="C41" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -993,7 +993,7 @@
         <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1006,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1019,7 +1019,7 @@
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1045,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -1071,7 +1071,7 @@
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1149,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1162,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -1292,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67">
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1344,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -1422,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77">
@@ -1448,7 +1448,7 @@
         <v>1</v>
       </c>
       <c r="C78" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79">
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -1487,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="C81" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1500,7 +1500,7 @@
         <v>2</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83">
@@ -1526,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85">
@@ -1539,7 +1539,7 @@
         <v>2</v>
       </c>
       <c r="C85" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86">
@@ -1565,7 +1565,7 @@
         <v>1</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88">
@@ -1591,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90">
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91">
@@ -1643,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94">
@@ -1656,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -1669,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -1708,7 +1708,7 @@
         <v>2</v>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99">
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -1773,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104">
@@ -1786,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105">
@@ -1799,7 +1799,7 @@
         <v>2</v>
       </c>
       <c r="C105" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106">
@@ -1812,7 +1812,7 @@
         <v>0</v>
       </c>
       <c r="C106" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107">
@@ -1890,7 +1890,7 @@
         <v>1</v>
       </c>
       <c r="C112" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -1903,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="C113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">

</xml_diff>